<commit_message>
added dummy Al data
</commit_message>
<xml_diff>
--- a/element_database/element_properties_for_ML-my elements.xlsx
+++ b/element_database/element_properties_for_ML-my elements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/imac/Desktop/Research/Oliynyk/2023_Summer_Research/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/research-code/cif-cn-featurizer/cif-cn-featurizer/element_database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F412D75-6F5D-3E48-8C37-E97CCA18D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159C41A2-38CE-4A44-BC3E-01D234331410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19780" yWindow="3700" windowWidth="33120" windowHeight="18000" xr2:uid="{E80F96DC-52AB-4791-94F6-1393503AEC81}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{E80F96DC-52AB-4791-94F6-1393503AEC81}"/>
   </bookViews>
   <sheets>
     <sheet name="properties" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Symbol</t>
   </si>
@@ -240,6 +240,9 @@
   <si>
     <t>valence e total</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Al</t>
   </si>
 </sst>
 </file>
@@ -247,13 +250,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -261,26 +264,26 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -356,7 +359,7 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,11 +384,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -394,7 +397,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -402,14 +405,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,7 +428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -724,14 +727,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB34"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B35" sqref="B35:AB35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7" style="9" customWidth="1"/>
     <col min="2" max="5" width="9.1640625" customWidth="1"/>
@@ -747,7 +750,7 @@
     <col min="18" max="18" width="27.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="4" customFormat="1" ht="58" customHeight="1">
+    <row r="1" spans="1:28" s="4" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -833,7 +836,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="16">
+    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
@@ -919,7 +922,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="16">
+    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="16">
+    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1091,7 +1094,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="16">
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="16">
+    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="16">
+    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="16">
+    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1435,7 +1438,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="16">
+    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="16">
+    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="16">
+    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="16">
+    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="16">
+    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
@@ -1865,7 +1868,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="16">
+    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="16">
+    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="16">
+    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>15</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="16">
+    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>16</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="16">
+    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="16">
+    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>18</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="16">
+    <row r="20" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>19</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="16">
+    <row r="21" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>20</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="16">
+    <row r="22" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>21</v>
       </c>
@@ -2639,7 +2642,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="16">
+    <row r="23" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>22</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="16">
+    <row r="24" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>23</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="16">
+    <row r="25" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>24</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="16">
+    <row r="26" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>25</v>
       </c>
@@ -2983,7 +2986,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="16">
+    <row r="27" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
@@ -3069,7 +3072,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="16">
+    <row r="28" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>27</v>
       </c>
@@ -3155,7 +3158,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="16">
+    <row r="29" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>28</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>6900</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="16">
+    <row r="30" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>29</v>
       </c>
@@ -3327,7 +3330,7 @@
         <v>7700</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="16">
+    <row r="31" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>30</v>
       </c>
@@ -3413,7 +3416,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="16">
+    <row r="32" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>31</v>
       </c>
@@ -3499,7 +3502,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="17">
+    <row r="33" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>32</v>
       </c>
@@ -3585,7 +3588,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="17">
+    <row r="34" spans="1:28" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>33</v>
       </c>
@@ -3669,6 +3672,92 @@
       </c>
       <c r="AB34">
         <v>6000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="19">
+        <v>69.722999999999999</v>
+      </c>
+      <c r="C35" s="2">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2">
+        <v>4</v>
+      </c>
+      <c r="E35" s="2">
+        <v>13</v>
+      </c>
+      <c r="F35" s="2">
+        <v>74</v>
+      </c>
+      <c r="G35" s="3">
+        <v>13</v>
+      </c>
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>3</v>
+      </c>
+      <c r="J35" s="12">
+        <v>2.6549999999999998</v>
+      </c>
+      <c r="K35" s="12">
+        <v>5.9992999999999999</v>
+      </c>
+      <c r="L35" s="22">
+        <v>7</v>
+      </c>
+      <c r="M35" s="14">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="N35" s="14">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="O35" s="24">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="P35" s="24">
+        <v>1.4079999999999999</v>
+      </c>
+      <c r="Q35" s="25">
+        <v>1.81</v>
+      </c>
+      <c r="R35" s="25">
+        <v>1.7</v>
+      </c>
+      <c r="S35" s="16">
+        <v>302.95</v>
+      </c>
+      <c r="T35" s="16">
+        <v>5.9</v>
+      </c>
+      <c r="U35" s="16">
+        <v>0.37</v>
+      </c>
+      <c r="V35" s="16">
+        <v>2.81</v>
+      </c>
+      <c r="W35" s="16">
+        <v>56.9</v>
+      </c>
+      <c r="X35">
+        <v>1.9397443490371991E-5</v>
+      </c>
+      <c r="Y35">
+        <v>1.232701287110975E-9</v>
+      </c>
+      <c r="Z35" s="20">
+        <v>5500</v>
+      </c>
+      <c r="AA35" s="20">
+        <v>1895</v>
+      </c>
+      <c r="AB35">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>